<commit_message>
chore: Suppression vieille photos et ajout nouvelles photos
</commit_message>
<xml_diff>
--- a/resultats_oiseaux.xlsx
+++ b/resultats_oiseaux.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,91 +453,1462 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>29032024-_L5A9943-Avec accentuation-Bruit-Modifier.jpg</t>
+          <t>01022024-_L5A6890-Avec accentuation-Bruit.jpg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Moineau domestique</t>
+          <t>Buse variable</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>85.06</v>
+        <v>58.74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>29102023-369A2792-Avec accentuation-Bruit.jpg</t>
+          <t>01032024-_L5A7791-Modifier.jpg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bergeronnette des ruisseaux</t>
+          <t>Goéland leucophée</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>86.89</v>
+        <v>49.65</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>31032024-369A3181-Modifier-Modifier.jpg</t>
+          <t>01032024-_L5A8034-Modifier.jpg</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tarier africain</t>
+          <t>Aigrette garzette</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>33.32</v>
+        <v>79.66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>31032024-369A3215.jpg</t>
+          <t>01032024-_L5A8139-Avec accentuation-Bruit.jpg</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Étourneau sansonnet</t>
+          <t>Cochevis huppé</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>65.73</v>
+        <v>60.57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>31032024-_L5A0274-Modifier.jpg</t>
+          <t>01032024-_L5A8174-Avec accentuation-Bruit.jpg</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tarier pâtre</t>
+          <t>Goéland leucophée</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>48.43</v>
+        <v>36.57</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>02032024-_L5A8194.jpg</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Pluvier doré</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>02032024-_L5A8719-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ibis falcinelle</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>20.85</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>02032024-_L5A8768-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Héron garde-boeufs</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>31.13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>03062024-_L5A3944-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Grand Cormoran</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>03062024-_L5A4005-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Goéland argenté</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>24.01</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04032024-_L5A9074.jpg</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Pluvier argenté</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>04062024-_L5A4165-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Fou de Bassan</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>22.06</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>05052024-_L5A2001-Modifier-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Pie d'Amérique</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>44.61</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>10062024-_L5A5173-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Héron cendré</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>72.31999999999999</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>10062024-_L5A5366-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Goéland argenté</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>38.72</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>14102023-369A0484-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Grande Aigrette</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>15052024-_L5A2674-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Pie bavarde</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>69.38</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>15102023-369A0635-2.jpg</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Martinet des maisons</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>29.93</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>16032024-_L5A9446-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Buse variable</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>67.51000000000001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>16102023-369A1463.jpg</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Héron garde-boeufs</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>78.77</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>17102023-369A2029-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Grande Aigrette</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>46.28</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>17112023-_L5A0835-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Goéland leucophée</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>43.74</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>18022024-_L5A7125-Avec accentuation-Bruit-topaz-denoise-sharpen.jpg</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Faucon crécerelle</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>65.08</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>22112023-_L5A1780-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Canard colvert</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>78.25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>23022024-_L5A7288-Avec accentuation-Bruit-Modifier-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Faucon crécerelle</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>24032024-_L5A9830-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Cormoran huppé</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>17.73</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>25052024-_L5A3712-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Grimpereau des jardins</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>75.11</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>26012024-_L5A6566-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Épervier d'Europe</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>52.73</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>31032024-369A3181-Modifier-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Tarier africain</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>33.32</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>31032024-369A3215.jpg</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Étourneau sansonnet</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>65.73</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>31032024-_L5A0274-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Tarier pâtre</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>48.43</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>369A0093-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Moineau domestique</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>369A0349-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Héron cendré</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>62.08</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>369A0431.jpg</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Mouette rieuse</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>41.8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>369A0476-2.jpg</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Flamant nain</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>20.45</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>369A0598.jpg</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Aigrette garzette</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>61.78</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>369A0681.jpg</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Héron garde-boeufs</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>61.41</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>369A0857.jpg</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Flamant rose</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>77.26000000000001</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>369A1224-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Grande Aigrette</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>72.53</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>369A1235-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Grande Aigrette</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>73.31</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>369A1252-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Grande Aigrette</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>63.96</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>369A1285.jpg</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Grande Aigrette</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>61.79</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>369A1374-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Grande Aigrette</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>65.16</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>369A1379-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Garde-boeufs d'Asie</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>17.25</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>369A1860-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Grand Cormoran</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>76.01000000000001</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>369A2087.jpg</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Faucon crécerelle</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>58.84</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>369A2092.jpg</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Faucon crécerellette</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>60.57</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>369A2116.jpg</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Oie des neiges</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>369A3316-Avec-accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Goéland leucophée</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>60.27</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>369A4697-Avec-accentuation-Bruit-DeNoiseAI-low-light-SharpenAI-motion.jpg</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Rougegorge familier</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>42.7</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>369A4824.jpg</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Faucon crécerelle</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>43.45</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>369A4846.jpg</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Faucon crécerelle</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>50.23</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>369A4847.jpg</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Faucon crécerelle</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>68.09</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>369A4883-Avec-accentuation-Bruit-SharpenAI-focus.jpg</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Bécasseau sanderling</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>369A4956-3-Avec-accentuation-Bruit-DeNoiseAI-low-light.jpg</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Hibou moyen-duc</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>79.40000000000001</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>369A5968-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Moineau domestique</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>67.41</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>369A6012-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Vautour fauve</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>369A6017-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Étourneau sansonnet</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>369A6019-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Pas de coords</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Pas de coords</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>369A6383-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Moineau domestique</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>60.44</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>369A6419-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Pas de coords</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Pas de coords</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>369A6442-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Harelde boréale</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>12.82</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>369A6444-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Foulque macroule</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>25.62</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>369A6447-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Foulque macroule</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>45.69</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>369A6720-denoise-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Canard souchet</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>59.58</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>369A6734-denoiselow-light.jpg</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Canard colvert</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>75.26000000000001</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>369A6817-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Tarier pâtre</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>51.62</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>369A7092-DeNoiseAI-low-light.jpg</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Grande Aigrette</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>61.76</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>369A7178-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Pic épeiche</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>63.91</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>369A7351-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Héron cendré</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>78.7</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>369A7383-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Grand Héron</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>27.01</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>369A7413-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Épervier à pieds courts</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>369A7491-2-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Busard pâle</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>44.53</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>369A7499-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Busard Saint-Martin</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>57.22</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>369A7574-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Mouette pygmée</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>17.65</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>369A7627-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Rossignol philomèle</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>40.96</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>369A7646-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Rossignol philomèle</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>7.43</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>369A7689.jpg</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Buse variable</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>46.83</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>369A7750-SharpenAI-motion.jpg</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Héron cendré</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>65.56</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>369A7757-DeNoiseAI-low-light.jpg</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Héron cendré</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>39.31</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>369A7859-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Pic épeiche</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>34.13</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>369A8370-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Troglodyte mignon</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>51.73</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>369A8373-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Troglodyte mignon</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>32.3</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>369A8689-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Canard noir</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>41.21</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>369A8862-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Pas de coords</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Pas de coords</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>369A9047-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Martin-pêcheur d'Amérique</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>369A9084-DeNoiseAI-clear.jpg</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Bergeronnette des ruisseaux</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>70.86</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>369A9185-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Canard colvert</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>27.14</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>369A9396-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Buse variable</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>71.55</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>369A9658-DeNoiseAI-low-light.jpg</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Grand Cormoran</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>79.62</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>369A9771-Avec accentuation-Bruit.jpg</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Cygne chanteur</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>33.08</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>369A9788.jpg</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Oie des moissons</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>13.61</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>369A9878.jpg</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Cygne tuberculé</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>59.52</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
           <t>Lythria cruentaria.jpg</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B95" t="inlineStr">
         <is>
           <t>Rousserolle turdoïde</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C95" t="n">
         <v>3.52</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>_L5A4572-Avec accentuation-Bruit-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Pouillot véloce</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>69.42</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>_L5A5578-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Troglodyte mignon</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>56.17</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>_L5A5798-Modifier.jpg</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Faucon hobereau</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>0.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>